<commit_message>
firstNum still displays after math operation
</commit_message>
<xml_diff>
--- a/State_Management - Calculator.xlsx
+++ b/State_Management - Calculator.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Action</t>
   </si>
@@ -45,30 +45,18 @@
     <t>null</t>
   </si>
   <si>
-    <t>firstNumberDisplay()</t>
-  </si>
-  <si>
     <t>Sequence of Steps</t>
   </si>
   <si>
-    <t>nothing</t>
-  </si>
-  <si>
     <t>Press No. '7'</t>
   </si>
   <si>
     <t>handleNumberPress called with '7' arg</t>
   </si>
   <si>
-    <t>Since length &lt; 9, set firstNumber to (' ' + ' 7')</t>
-  </si>
-  <si>
     <t>"7"</t>
   </si>
   <si>
-    <t>state change</t>
-  </si>
-  <si>
     <t>Press operation '*'</t>
   </si>
   <si>
@@ -81,24 +69,15 @@
     <t>"*"</t>
   </si>
   <si>
-    <t>firstNumberDisplay() called - DONE</t>
-  </si>
-  <si>
     <t>Next, press No. '2'</t>
   </si>
   <si>
     <t>handleNumberPress called with '2' arg</t>
   </si>
   <si>
-    <t>Since length &lt; 9, set firstNumber to ('7 ' + ' 2')</t>
-  </si>
-  <si>
     <t>"72"</t>
   </si>
   <si>
-    <t>Final state change: re-render - DONE</t>
-  </si>
-  <si>
     <t xml:space="preserve">setFirstNumber to " " </t>
   </si>
   <si>
@@ -123,7 +102,34 @@
     <t>nextDigit</t>
   </si>
   <si>
-    <t xml:space="preserve">54               3 </t>
+    <t>Since firstNumber currently set to '', then this &lt; 12</t>
+  </si>
+  <si>
+    <t>Therefore change state: setFirstNumber to (' ' + ' 7')</t>
+  </si>
+  <si>
+    <t>secondNumber displayed</t>
+  </si>
+  <si>
+    <t>firstNumberDisplay() results</t>
+  </si>
+  <si>
+    <t>state change and a render occurs</t>
+  </si>
+  <si>
+    <t>firstNumberDisplay() called</t>
+  </si>
+  <si>
+    <t>Since length firstNumber &lt; 12 (curently '7'), set firstNumber to ('7 ' + ' 2')</t>
+  </si>
+  <si>
+    <t>state change and render occurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstNumberDisplay() called </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final state change: re-render </t>
   </si>
 </sst>
 </file>
@@ -521,20 +527,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="57.7109375" customWidth="1"/>
+    <col min="2" max="2" width="65.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" style="2" customWidth="1"/>
     <col min="5" max="6" width="12.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -543,7 +549,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -558,10 +564,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -584,15 +590,15 @@
         <v>0</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -603,9 +609,9 @@
     </row>
     <row r="4" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -614,7 +620,7 @@
     </row>
     <row r="5" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
@@ -625,38 +631,33 @@
     </row>
     <row r="6" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>15</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C6" s="6"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="6"/>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -665,137 +666,143 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
       <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+        <v>18</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>25</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="A13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11">
+      <c r="D17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11">
         <v>0</v>
       </c>
-      <c r="H16" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -804,26 +811,26 @@
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -846,20 +853,20 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="C24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -880,6 +887,14 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add dark and light mode Ionic icons to Switch
</commit_message>
<xml_diff>
--- a/State_Management - Calculator.xlsx
+++ b/State_Management - Calculator.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>Action</t>
   </si>
@@ -130,13 +130,97 @@
   </si>
   <si>
     <t xml:space="preserve">Final state change: re-render </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ' + '7"</t>
+  </si>
+  <si>
+    <t>Scenarios for pressing a number:</t>
+  </si>
+  <si>
+    <t>operation?</t>
+  </si>
+  <si>
+    <t>secondNumber?</t>
+  </si>
+  <si>
+    <t>result?</t>
+  </si>
+  <si>
+    <t>firstNumber?</t>
+  </si>
+  <si>
+    <t>Scenarios for pressing operation?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstNumber? </t>
+  </si>
+  <si>
+    <t>Desired result?</t>
+  </si>
+  <si>
+    <t>Then to concatenate current 'title' with existing firstNumber</t>
+  </si>
+  <si>
+    <t>Then next number press is the start of the next 'secondNumber'</t>
+  </si>
+  <si>
+    <t>Same as firstNumber: o concatenate current 'title' with existing secondNumber</t>
+  </si>
+  <si>
+    <t>Begins a brand new operation and new button press is start of new firstNumber</t>
+  </si>
+  <si>
+    <t>handleNumberPress()</t>
+  </si>
+  <si>
+    <t>[firstNumber, setFirstNumber]</t>
+  </si>
+  <si>
+    <t>[secondNumber, setSecondNumber]</t>
+  </si>
+  <si>
+    <t>[operation, setOperation]</t>
+  </si>
+  <si>
+    <t>[result, setResult]</t>
+  </si>
+  <si>
+    <t>handleOperationPress()</t>
+  </si>
+  <si>
+    <t>handlePercentPress()</t>
+  </si>
+  <si>
+    <t>clear()</t>
+  </si>
+  <si>
+    <t>getResult()</t>
+  </si>
+  <si>
+    <t>firstNumberDisplay()</t>
+  </si>
+  <si>
+    <t>{secondNumber}</t>
+  </si>
+  <si>
+    <t>{firstNumberDisplay()}</t>
+  </si>
+  <si>
+    <t>1+2+3+4+5</t>
+  </si>
+  <si>
+    <t>setFirstNumber(' ' + ' 7)</t>
+  </si>
+  <si>
+    <t>'7'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,8 +252,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +273,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -192,10 +288,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -226,8 +323,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,15 +628,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
     <col min="2" max="2" width="65.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" style="2" customWidth="1"/>
@@ -598,20 +699,29 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -619,9 +729,6 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -630,9 +737,6 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -641,21 +745,12 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="C7" s="6"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="6"/>
@@ -667,76 +762,97 @@
     </row>
     <row r="9" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
       <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
       <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
       <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>19</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C12" s="6"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-    </row>
     <row r="14" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -745,65 +861,45 @@
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
       <c r="C15" s="6"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
       <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11">
-        <v>0</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>22</v>
-      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
       <c r="B18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="C18" s="6"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -811,33 +907,40 @@
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="3"/>
+      <c r="A19" s="7"/>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="A20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="3"/>
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="6"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -845,34 +948,64 @@
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="3"/>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="6"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="G23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11">
+        <v>0</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -889,12 +1022,82 @@
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -904,24 +1107,152 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="73.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A4:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>